<commit_message>
Added data from Safety, Security and Fire Reports 2012-2018
</commit_message>
<xml_diff>
--- a/Formatted-Data/raw_released_data.xlsx
+++ b/Formatted-Data/raw_released_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\Documents\alc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\Documents\alc\Formatted-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50BEDB2-2D21-4E78-824A-FE848DEE6511}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFA6040-044A-4B38-A42A-5BD8EA989772}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{AC0BD6E1-1E93-43A4-8FE7-90504166469E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{AC0BD6E1-1E93-43A4-8FE7-90504166469E}"/>
   </bookViews>
   <sheets>
     <sheet name="FROSH SURVEY RESULTS, 2012-2018" sheetId="1" r:id="rId1"/>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B93501D-9FFD-431F-A6B0-5767EF8CA38F}">
   <dimension ref="A1:I142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4468,8 +4468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFAE440-41FB-4F7D-B135-076641C121EA}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:A39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5762,13 +5762,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42980F8A-CB6F-4C48-AF4B-C4BD3721079F}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="60.85546875" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>